<commit_message>
No memory leaks finally.
</commit_message>
<xml_diff>
--- a/documentation/general_information/Budget.xlsx
+++ b/documentation/general_information/Budget.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -55,16 +55,28 @@
     <t xml:space="preserve">Carlos</t>
   </si>
   <si>
+    <t xml:space="preserve">Progressive Automation PA-15-4-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progressive Automation PA-15-4-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA-15 Bracket Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peer Bearing 1641-2RS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wires</t>
   </si>
   <si>
-    <t xml:space="preserve">Eliel</t>
-  </si>
-  <si>
     <t xml:space="preserve">Miscellanous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jordan</t>
   </si>
   <si>
     <t xml:space="preserve">Spools</t>
@@ -149,13 +161,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -175,32 +191,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.4744897959184"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>4</v>
       </c>
     </row>
@@ -208,154 +224,215 @@
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="C2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="D2" s="1" t="n">
         <v>16.95</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <f aca="false">B2*C2</f>
+      <c r="E2" s="1" t="n">
+        <f aca="false">C2*D2</f>
         <v>50.85</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <f aca="false">C2*1+6.45</f>
-        <v>23.4</v>
-      </c>
       <c r="H2" s="1" t="n">
-        <f aca="false">D10-G2</f>
-        <v>295.566</v>
+        <f aca="false">D2+6.45+E7+E8</f>
+        <v>211.32</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <f aca="false">E14-H2</f>
+        <v>101.63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="D3" s="1" t="n">
         <v>21.99</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <f aca="false">B3*C3</f>
+      <c r="E3" s="1" t="n">
+        <f aca="false">C3*D3</f>
         <v>43.98</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <f aca="false">C3*2</f>
-        <v>43.98</v>
-      </c>
       <c r="H3" s="1" t="n">
-        <f aca="false">D10-G3</f>
-        <v>274.986</v>
+        <f aca="false">D3*2+E11</f>
+        <v>283.98</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <f aca="false">E14-H3</f>
+        <v>28.97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="n">
+        <f aca="false">E14-H4</f>
+        <v>312.95</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <f aca="false">C5*D5</f>
+        <v>314</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="n">
+        <f aca="false">E14-H5</f>
+        <v>312.95</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <f aca="false">C6*D6</f>
+        <v>628</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="n">
+        <f aca="false">E14-H6</f>
+        <v>312.95</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <f aca="false">B4*C4</f>
-        <v>1200</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="D7" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <f aca="false">C7*D7</f>
+        <v>102</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <f aca="false">C8*D8</f>
+        <v>85.92</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <f aca="false">C9*D9</f>
+        <v>40</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="n">
-        <f aca="false">D10-G4</f>
-        <v>318.966</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <f aca="false">B5*C5</f>
-        <v>40</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="n">
-        <f aca="false">D10-G5</f>
-        <v>318.966</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <f aca="false">B6*C6</f>
+      <c r="E10" s="1" t="n">
+        <f aca="false">C10*D10</f>
         <v>60</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="n">
-        <f aca="false">D10-G6</f>
-        <v>318.966</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <f aca="false">B7*C7</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <f aca="false">SUM(D2:D7)</f>
-        <v>1594.83</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <f aca="false">D9/5</f>
-        <v>318.966</v>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <f aca="false">C11*D11</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <f aca="false">SUM(E2:E11)</f>
+        <v>1564.75</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <f aca="false">E13/5</f>
+        <v>312.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added boost threads and some other small details.
</commit_message>
<xml_diff>
--- a/documentation/general_information/Budget.xlsx
+++ b/documentation/general_information/Budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -194,13 +194,14 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -225,14 +226,14 @@
         <v>5</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>16.95</v>
       </c>
       <c r="E2" s="1" t="n">
         <f aca="false">C2*D2</f>
-        <v>50.85</v>
+        <v>84.75</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>6</v>
@@ -243,7 +244,7 @@
       </c>
       <c r="I2" s="1" t="n">
         <f aca="false">E14-H2</f>
-        <v>101.63</v>
+        <v>166.01</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,11 +266,11 @@
       </c>
       <c r="H3" s="1" t="n">
         <f aca="false">D3*2+E11</f>
-        <v>283.98</v>
+        <v>571.98</v>
       </c>
       <c r="I3" s="1" t="n">
         <f aca="false">E14-H3</f>
-        <v>28.97</v>
+        <v>-194.65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,7 +285,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="n">
         <f aca="false">E14-H4</f>
-        <v>312.95</v>
+        <v>377.33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,7 +308,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="n">
         <f aca="false">E14-H5</f>
-        <v>312.95</v>
+        <v>377.33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -330,7 +331,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="n">
         <f aca="false">E14-H6</f>
-        <v>312.95</v>
+        <v>377.33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,14 +408,14 @@
         <v>19</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>48</v>
       </c>
       <c r="E11" s="1" t="n">
         <f aca="false">C11*D11</f>
-        <v>240</v>
+        <v>528</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,7 +424,7 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="false">SUM(E2:E11)</f>
-        <v>1564.75</v>
+        <v>1886.65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,7 +433,7 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="false">E13/5</f>
-        <v>312.95</v>
+        <v>377.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a wring diagram for the pi, gyro, and ir sensor together.
</commit_message>
<xml_diff>
--- a/documentation/general_information/Budget.xlsx
+++ b/documentation/general_information/Budget.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">Raspberry pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PerfBorad, PCB Standoff, Female Pin Headers, IR Sensor</t>
   </si>
   <si>
     <t xml:space="preserve">total</t>
@@ -212,16 +215,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -266,8 +270,8 @@
         <v>301.6</v>
       </c>
       <c r="J2" s="1" t="n">
-        <f aca="false">F21-I2</f>
-        <v>77.586</v>
+        <f aca="false">F22-I2</f>
+        <v>85.682</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,12 +295,12 @@
         <v>10</v>
       </c>
       <c r="I3" s="1" t="n">
-        <f aca="false">E3*2+F13+F11+F12+F5+F6-485.48</f>
-        <v>376.49</v>
+        <f aca="false">E3*2+F13+F11+F12+F5+F6-485.48+F19</f>
+        <v>416.97</v>
       </c>
       <c r="J3" s="1" t="n">
-        <f aca="false">F21-I3</f>
-        <v>2.69600000000003</v>
+        <f aca="false">F22-I3</f>
+        <v>-29.688</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,8 +319,8 @@
         <v>376.49</v>
       </c>
       <c r="J4" s="1" t="n">
-        <f aca="false">F21-I4</f>
-        <v>2.69600000000003</v>
+        <f aca="false">F22-I4</f>
+        <v>10.792</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,8 +347,8 @@
         <v>400</v>
       </c>
       <c r="J5" s="1" t="n">
-        <f aca="false">F21-I5</f>
-        <v>-20.814</v>
+        <f aca="false">F22-I5</f>
+        <v>-12.718</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -368,8 +372,8 @@
         <v>380</v>
       </c>
       <c r="J6" s="1" t="n">
-        <f aca="false">F21-I6</f>
-        <v>-0.813999999999965</v>
+        <f aca="false">F22-I6</f>
+        <v>7.28200000000004</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,24 +599,42 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="1"/>
+      <c r="A19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>40.48</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">D19*E19</f>
+        <v>40.48</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="1" t="n">
-        <f aca="false">SUM(F2:F18)</f>
-        <v>1895.93</v>
-      </c>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="0" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="1" t="n">
-        <f aca="false">F20/5</f>
-        <v>379.186</v>
+        <f aca="false">SUM(F2:F19)</f>
+        <v>1936.41</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <f aca="false">F21/5</f>
+        <v>387.282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>